<commit_message>
minor changes to dialogu list
</commit_message>
<xml_diff>
--- a/Results/adversarial_attack/evidence_test_meta.llama2-70b-chat-v122febtest.xlsx
+++ b/Results/adversarial_attack/evidence_test_meta.llama2-70b-chat-v122febtest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GAMES_SETUP\Thesis\Code\Results\adversarial_attack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E796D5-B096-4C42-A880-DA26F8ACD436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6EC650-1147-4693-9F04-93CD95B607FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="475">
   <si>
     <t>ques_id</t>
   </si>
@@ -1420,12 +1420,6 @@
     <t>Uncertainty</t>
   </si>
   <si>
-    <t>Knowledge</t>
-  </si>
-  <si>
-    <t>Unknowledge</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -1442,13 +1436,22 @@
   </si>
   <si>
     <t>Correct response remains consistent</t>
+  </si>
+  <si>
+    <t>Knowledgeable</t>
+  </si>
+  <si>
+    <t>Unknowledgeable</t>
+  </si>
+  <si>
+    <t>Incorrect response remains or keeps fluctuating</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1478,8 +1481,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1494,6 +1511,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -1521,22 +1549,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1839,13 +1873,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N107"/>
+  <dimension ref="A1:Q107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -3527,7 +3565,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -3562,7 +3600,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -3597,7 +3635,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -3632,17 +3670,17 @@
         <v>455</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>456</v>
       </c>
@@ -3653,7 +3691,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>457</v>
       </c>
@@ -3661,114 +3699,138 @@
         <v>458</v>
       </c>
       <c r="C57" t="s">
+        <v>466</v>
+      </c>
+      <c r="H57" t="s">
+        <v>472</v>
+      </c>
+      <c r="I57" s="2">
+        <v>31</v>
+      </c>
+      <c r="J57" s="4">
+        <v>5</v>
+      </c>
+      <c r="P57" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="H57" t="s">
-        <v>466</v>
-      </c>
-      <c r="I57">
-        <v>31</v>
-      </c>
-      <c r="J57">
-        <v>5</v>
-      </c>
-      <c r="M57" t="s">
-        <v>470</v>
-      </c>
-      <c r="N57" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q57" s="4" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>2</v>
       </c>
       <c r="B58" t="s">
         <v>460</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="H58" t="s">
+        <v>473</v>
+      </c>
+      <c r="I58" s="5">
+        <v>6</v>
+      </c>
+      <c r="J58" s="3">
+        <v>8</v>
+      </c>
+      <c r="P58" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="H58" t="s">
-        <v>467</v>
-      </c>
-      <c r="I58">
-        <v>6</v>
-      </c>
-      <c r="J58">
-        <v>8</v>
-      </c>
-      <c r="M58" t="s">
-        <v>471</v>
-      </c>
-      <c r="N58" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="Q58" s="3" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>4</v>
       </c>
       <c r="B59" t="s">
         <v>459</v>
       </c>
-      <c r="C59" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C59" s="3" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>10</v>
       </c>
       <c r="B60" t="s">
         <v>460</v>
       </c>
-      <c r="C60" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C60" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="I60" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>12</v>
       </c>
       <c r="B61" t="s">
         <v>461</v>
       </c>
-      <c r="C61" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C61" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="I61" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>13</v>
       </c>
       <c r="B62" t="s">
         <v>459</v>
       </c>
-      <c r="C62" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C62" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="I62" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>15</v>
       </c>
       <c r="B63" t="s">
         <v>460</v>
       </c>
-      <c r="C63" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C63" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="I63" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>17</v>
       </c>
       <c r="B64" t="s">
         <v>459</v>
       </c>
-      <c r="C64" t="s">
-        <v>472</v>
+      <c r="C64" s="3" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -3778,8 +3840,8 @@
       <c r="B65" t="s">
         <v>459</v>
       </c>
-      <c r="C65" t="s">
-        <v>472</v>
+      <c r="C65" s="3" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -3789,8 +3851,8 @@
       <c r="B66" t="s">
         <v>460</v>
       </c>
-      <c r="C66" t="s">
-        <v>469</v>
+      <c r="C66" s="4" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -3800,8 +3862,8 @@
       <c r="B67" t="s">
         <v>459</v>
       </c>
-      <c r="C67" t="s">
-        <v>472</v>
+      <c r="C67" s="3" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -3811,8 +3873,8 @@
       <c r="B68" t="s">
         <v>460</v>
       </c>
-      <c r="C68" t="s">
-        <v>469</v>
+      <c r="C68" s="4" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -3822,8 +3884,8 @@
       <c r="B69" t="s">
         <v>461</v>
       </c>
-      <c r="C69" t="s">
-        <v>471</v>
+      <c r="C69" s="5" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -3833,8 +3895,8 @@
       <c r="B70" t="s">
         <v>461</v>
       </c>
-      <c r="C70" t="s">
-        <v>471</v>
+      <c r="C70" s="5" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -3844,8 +3906,8 @@
       <c r="B71" t="s">
         <v>459</v>
       </c>
-      <c r="C71" t="s">
-        <v>472</v>
+      <c r="C71" s="3" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -3855,8 +3917,8 @@
       <c r="B72" t="s">
         <v>461</v>
       </c>
-      <c r="C72" t="s">
-        <v>471</v>
+      <c r="C72" s="5" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
@@ -3866,8 +3928,8 @@
       <c r="B73" t="s">
         <v>459</v>
       </c>
-      <c r="C73" t="s">
-        <v>472</v>
+      <c r="C73" s="3" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
@@ -3877,8 +3939,8 @@
       <c r="B74" t="s">
         <v>461</v>
       </c>
-      <c r="C74" t="s">
-        <v>471</v>
+      <c r="C74" s="5" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -3888,8 +3950,8 @@
       <c r="B75" t="s">
         <v>459</v>
       </c>
-      <c r="C75" t="s">
-        <v>472</v>
+      <c r="C75" s="3" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -3899,8 +3961,8 @@
       <c r="B76" t="s">
         <v>461</v>
       </c>
-      <c r="C76" t="s">
-        <v>471</v>
+      <c r="C76" s="5" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -3908,10 +3970,10 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C77" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -3919,10 +3981,10 @@
         <v>1</v>
       </c>
       <c r="B78" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C78" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -3930,10 +3992,10 @@
         <v>3</v>
       </c>
       <c r="B79" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C79" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -3941,10 +4003,10 @@
         <v>5</v>
       </c>
       <c r="B80" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C80" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -3952,10 +4014,10 @@
         <v>6</v>
       </c>
       <c r="B81" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C81" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -3963,10 +4025,10 @@
         <v>7</v>
       </c>
       <c r="B82" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C82" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -3974,10 +4036,10 @@
         <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C83" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -3985,10 +4047,10 @@
         <v>9</v>
       </c>
       <c r="B84" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C84" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -3996,10 +4058,10 @@
         <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C85" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -4007,10 +4069,10 @@
         <v>14</v>
       </c>
       <c r="B86" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C86" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -4018,10 +4080,10 @@
         <v>16</v>
       </c>
       <c r="B87" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C87" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -4029,10 +4091,10 @@
         <v>18</v>
       </c>
       <c r="B88" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C88" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -4040,10 +4102,10 @@
         <v>19</v>
       </c>
       <c r="B89" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C89" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -4051,10 +4113,10 @@
         <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C90" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -4062,10 +4124,10 @@
         <v>22</v>
       </c>
       <c r="B91" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C91" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -4073,10 +4135,10 @@
         <v>24</v>
       </c>
       <c r="B92" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C92" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -4084,10 +4146,10 @@
         <v>26</v>
       </c>
       <c r="B93" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C93" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
@@ -4095,10 +4157,10 @@
         <v>27</v>
       </c>
       <c r="B94" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C94" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
@@ -4106,10 +4168,10 @@
         <v>28</v>
       </c>
       <c r="B95" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C95" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
@@ -4117,10 +4179,10 @@
         <v>29</v>
       </c>
       <c r="B96" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C96" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
@@ -4128,10 +4190,10 @@
         <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C97" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
@@ -4139,10 +4201,10 @@
         <v>33</v>
       </c>
       <c r="B98" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C98" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
@@ -4150,10 +4212,10 @@
         <v>34</v>
       </c>
       <c r="B99" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C99" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
@@ -4161,10 +4223,10 @@
         <v>35</v>
       </c>
       <c r="B100" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C100" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
@@ -4172,10 +4234,10 @@
         <v>36</v>
       </c>
       <c r="B101" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C101" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
@@ -4183,10 +4245,10 @@
         <v>38</v>
       </c>
       <c r="B102" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C102" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
@@ -4194,10 +4256,10 @@
         <v>41</v>
       </c>
       <c r="B103" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C103" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
@@ -4205,10 +4267,10 @@
         <v>42</v>
       </c>
       <c r="B104" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C104" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
@@ -4216,10 +4278,10 @@
         <v>44</v>
       </c>
       <c r="B105" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C105" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
@@ -4227,10 +4289,10 @@
         <v>45</v>
       </c>
       <c r="B106" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C106" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
@@ -4238,10 +4300,10 @@
         <v>47</v>
       </c>
       <c r="B107" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C107" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>